<commit_message>
UwU Gravity is here
</commit_message>
<xml_diff>
--- a/Momente.xlsx
+++ b/Momente.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calculation" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Calculation" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +472,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9065.507351940967</v>
+        <v>5489.077381324905</v>
       </c>
       <c r="B2" t="n">
-        <v>90655.07351940966</v>
+        <v>164084.9901599454</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>29.893</v>
       </c>
       <c r="D2" t="n">
-        <v>-45327.53675970483</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -495,19 +495,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>640.6634487247856</v>
+        <v>837.2059528526869</v>
       </c>
       <c r="B3" t="n">
-        <v>32033.17243623928</v>
+        <v>26552.82400067582</v>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>31.716</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>-1046.507441065859</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -518,24 +518,461 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34303.69336799387</v>
+        <v>589.7202104509649</v>
       </c>
       <c r="B4" t="n">
-        <v>857592.3341998467</v>
+        <v>18703.56619466281</v>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>31.716</v>
       </c>
       <c r="D4" t="n">
-        <v>68607.38673598773</v>
+        <v>-737.1502630637062</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>-1.25</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>934.4551556770092</v>
+      </c>
+      <c r="B5" t="n">
+        <v>27933.66796865284</v>
+      </c>
+      <c r="C5" t="n">
+        <v>29.893</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1892.271690245944</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-2.025</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1078</v>
+      </c>
+      <c r="B6" t="n">
+        <v>30610.888</v>
+      </c>
+      <c r="C6" t="n">
+        <v>28.396</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1347.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>18131.67667630768</v>
+      </c>
+      <c r="B7" t="n">
+        <v>627356.0130002459</v>
+      </c>
+      <c r="C7" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>44603.92462371691</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>640.6634487247856</v>
+      </c>
+      <c r="B8" t="n">
+        <v>38079.11340185508</v>
+      </c>
+      <c r="C8" t="n">
+        <v>59.437</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3767.101078501739</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>34355.11037416998</v>
+      </c>
+      <c r="B9" t="n">
+        <v>969329.4392072061</v>
+      </c>
+      <c r="C9" t="n">
+        <v>28.215</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3435.511037416999</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>609.7648057024572</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3048.824028512286</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-2439.059222809829</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3632.315283511329</v>
+      </c>
+      <c r="B11" t="n">
+        <v>133542.071398294</v>
+      </c>
+      <c r="C11" t="n">
+        <v>36.765</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-14529.26113404532</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>874.1792747922477</v>
+      </c>
+      <c r="B12" t="n">
+        <v>33552.74892507605</v>
+      </c>
+      <c r="C12" t="n">
+        <v>38.382</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2149.606836714137</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>968.3975456496001</v>
+      </c>
+      <c r="B13" t="n">
+        <v>31614.30627527685</v>
+      </c>
+      <c r="C13" t="n">
+        <v>32.646</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2381.289564752367</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>968.3975456496001</v>
+      </c>
+      <c r="B14" t="n">
+        <v>34689.93688025998</v>
+      </c>
+      <c r="C14" t="n">
+        <v>35.822</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2381.289564752367</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3162.2887004064</v>
+      </c>
+      <c r="B15" t="n">
+        <v>100073.788213061</v>
+      </c>
+      <c r="C15" t="n">
+        <v>31.646</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7776.067914299339</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3162.2887004064</v>
+      </c>
+      <c r="B16" t="n">
+        <v>110117.2171255517</v>
+      </c>
+      <c r="C16" t="n">
+        <v>34.822</v>
+      </c>
+      <c r="D16" t="n">
+        <v>7776.067914299339</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1452.31617179842</v>
+      </c>
+      <c r="B17" t="n">
+        <v>10166.21320258894</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1452.31617179842</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>866.3</v>
+      </c>
+      <c r="B18" t="n">
+        <v>35403.08209999999</v>
+      </c>
+      <c r="C18" t="n">
+        <v>40.867</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1064.6827</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.229</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1455.253333333333</v>
+      </c>
+      <c r="B19" t="n">
+        <v>36547.23221333334</v>
+      </c>
+      <c r="C19" t="n">
+        <v>25.114</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-727.6266666666667</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3528.131515227642</v>
+      </c>
+      <c r="B20" t="n">
+        <v>105466.4353846999</v>
+      </c>
+      <c r="C20" t="n">
+        <v>29.893</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3528.131515227642</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>916.3566448633733</v>
+      </c>
+      <c r="B21" t="n">
+        <v>19243.48954213084</v>
+      </c>
+      <c r="C21" t="n">
+        <v>21</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1145.445806079217</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-1.25</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1728</v>
+      </c>
+      <c r="B22" t="n">
+        <v>65342.592</v>
+      </c>
+      <c r="C22" t="n">
+        <v>37.814</v>
+      </c>
+      <c r="D22" t="n">
+        <v>864</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>600</v>
+      </c>
+      <c r="B23" t="n">
+        <v>8194.799999999999</v>
+      </c>
+      <c r="C23" t="n">
+        <v>13.658</v>
+      </c>
+      <c r="D23" t="n">
+        <v>300</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed a Lot Might be completley Fucked but should theoretically all be good. UwU
</commit_message>
<xml_diff>
--- a/Momente.xlsx
+++ b/Momente.xlsx
@@ -590,10 +590,10 @@
         <v>18131.67667630768</v>
       </c>
       <c r="B7" t="n">
-        <v>627356.0130002459</v>
+        <v>554829.3062950152</v>
       </c>
       <c r="C7" t="n">
-        <v>34.6</v>
+        <v>30.6</v>
       </c>
       <c r="D7" t="n">
         <v>44603.92462371691</v>
@@ -728,10 +728,10 @@
         <v>968.3975456496001</v>
       </c>
       <c r="B13" t="n">
-        <v>31614.30627527685</v>
+        <v>27740.71609267845</v>
       </c>
       <c r="C13" t="n">
-        <v>32.646</v>
+        <v>28.646</v>
       </c>
       <c r="D13" t="n">
         <v>2381.289564752367</v>
@@ -751,10 +751,10 @@
         <v>968.3975456496001</v>
       </c>
       <c r="B14" t="n">
-        <v>34689.93688025998</v>
+        <v>30816.34669766158</v>
       </c>
       <c r="C14" t="n">
-        <v>35.822</v>
+        <v>31.822</v>
       </c>
       <c r="D14" t="n">
         <v>2381.289564752367</v>
@@ -774,10 +774,10 @@
         <v>3162.2887004064</v>
       </c>
       <c r="B15" t="n">
-        <v>100073.788213061</v>
+        <v>87424.63341143535</v>
       </c>
       <c r="C15" t="n">
-        <v>31.646</v>
+        <v>27.646</v>
       </c>
       <c r="D15" t="n">
         <v>7776.067914299339</v>
@@ -797,10 +797,10 @@
         <v>3162.2887004064</v>
       </c>
       <c r="B16" t="n">
-        <v>110117.2171255517</v>
+        <v>97468.06232392609</v>
       </c>
       <c r="C16" t="n">
-        <v>34.822</v>
+        <v>30.822</v>
       </c>
       <c r="D16" t="n">
         <v>7776.067914299339</v>

</xml_diff>